<commit_message>
Lo qe tengo hasta ahora.
</commit_message>
<xml_diff>
--- a/code/pruebas/Pruebas.xlsx
+++ b/code/pruebas/Pruebas.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="362" uniqueCount="118">
   <si>
     <t>PERSONA</t>
   </si>
@@ -367,6 +367,9 @@
   </si>
   <si>
     <t>23+5</t>
+  </si>
+  <si>
+    <t>Distancia</t>
   </si>
 </sst>
 </file>
@@ -757,7 +760,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="67">
+  <cellXfs count="70">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -853,12 +856,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,6 +942,21 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1265,10 +1277,10 @@
       <c r="H1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="I1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="J1" s="32"/>
+      <c r="I1" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="J1" s="65"/>
       <c r="L1" s="14" t="s">
         <v>0</v>
       </c>
@@ -1281,17 +1293,17 @@
       <c r="O1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="32"/>
+      <c r="P1" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="65"/>
       <c r="R1" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="S1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="T1" s="32"/>
+      <c r="S1" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="T1" s="65"/>
     </row>
     <row r="2" spans="7:20" s="16" customFormat="1" ht="15.75" thickBot="1">
       <c r="G2" s="14"/>
@@ -1328,7 +1340,7 @@
       <c r="G3" s="2">
         <v>3</v>
       </c>
-      <c r="H3" s="35">
+      <c r="H3" s="33">
         <v>29</v>
       </c>
       <c r="I3" s="20" t="s">
@@ -1346,7 +1358,7 @@
       <c r="N3" s="2">
         <v>5</v>
       </c>
-      <c r="O3" s="35">
+      <c r="O3" s="33">
         <v>28</v>
       </c>
       <c r="P3" s="20" t="s">
@@ -1363,7 +1375,7 @@
       <c r="G4" s="3">
         <v>3</v>
       </c>
-      <c r="H4" s="36">
+      <c r="H4" s="34">
         <v>29</v>
       </c>
       <c r="I4" s="28" t="s">
@@ -1381,7 +1393,7 @@
       <c r="N4" s="3">
         <v>5</v>
       </c>
-      <c r="O4" s="36"/>
+      <c r="O4" s="34"/>
       <c r="P4" s="28" t="s">
         <v>45</v>
       </c>
@@ -1396,7 +1408,7 @@
       <c r="G5" s="3">
         <v>3</v>
       </c>
-      <c r="H5" s="36">
+      <c r="H5" s="34">
         <v>28</v>
       </c>
       <c r="I5" s="26" t="s">
@@ -1414,7 +1426,7 @@
       <c r="N5" s="3">
         <v>5</v>
       </c>
-      <c r="O5" s="36"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="30" t="s">
         <v>73</v>
       </c>
@@ -1429,7 +1441,7 @@
       <c r="G6" s="3">
         <v>3</v>
       </c>
-      <c r="H6" s="36">
+      <c r="H6" s="34">
         <v>29</v>
       </c>
       <c r="I6" s="28" t="s">
@@ -1447,7 +1459,7 @@
       <c r="N6" s="3">
         <v>5</v>
       </c>
-      <c r="O6" s="36"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="28" t="s">
         <v>73</v>
       </c>
@@ -1462,7 +1474,7 @@
       <c r="G7" s="9">
         <v>3</v>
       </c>
-      <c r="H7" s="37"/>
+      <c r="H7" s="35"/>
       <c r="I7" s="22" t="s">
         <v>38</v>
       </c>
@@ -1478,7 +1490,7 @@
       <c r="N7" s="9">
         <v>5</v>
       </c>
-      <c r="O7" s="37"/>
+      <c r="O7" s="35"/>
       <c r="P7" s="22" t="s">
         <v>73</v>
       </c>
@@ -1493,11 +1505,11 @@
       <c r="G8" s="3">
         <v>3</v>
       </c>
-      <c r="H8" s="36"/>
-      <c r="I8" s="40" t="s">
+      <c r="H8" s="34"/>
+      <c r="I8" s="38" t="s">
         <v>59</v>
       </c>
-      <c r="J8" s="41" t="s">
+      <c r="J8" s="39" t="s">
         <v>54</v>
       </c>
       <c r="L8" s="6" t="s">
@@ -1509,22 +1521,22 @@
       <c r="N8" s="3">
         <v>5</v>
       </c>
-      <c r="O8" s="36"/>
-      <c r="P8" s="39" t="s">
+      <c r="O8" s="34"/>
+      <c r="P8" s="37" t="s">
         <v>73</v>
       </c>
-      <c r="Q8" s="54">
+      <c r="Q8" s="52">
         <v>1.0649999999999999</v>
       </c>
       <c r="R8" s="3"/>
-      <c r="S8" s="33"/>
-      <c r="T8" s="34"/>
+      <c r="S8" s="66"/>
+      <c r="T8" s="67"/>
     </row>
     <row r="9" spans="7:20">
       <c r="G9" s="3">
         <v>3</v>
       </c>
-      <c r="H9" s="36"/>
+      <c r="H9" s="34"/>
       <c r="I9" s="28" t="s">
         <v>60</v>
       </c>
@@ -1540,7 +1552,7 @@
       <c r="N9" s="3">
         <v>5</v>
       </c>
-      <c r="O9" s="36"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="28" t="s">
         <v>56</v>
       </c>
@@ -1555,7 +1567,7 @@
       <c r="G10" s="3">
         <v>3</v>
       </c>
-      <c r="H10" s="36"/>
+      <c r="H10" s="34"/>
       <c r="I10" s="28" t="s">
         <v>61</v>
       </c>
@@ -1571,7 +1583,7 @@
       <c r="N10" s="3">
         <v>5</v>
       </c>
-      <c r="O10" s="36"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="28" t="s">
         <v>103</v>
       </c>
@@ -1586,7 +1598,7 @@
       <c r="G11" s="3">
         <v>3</v>
       </c>
-      <c r="H11" s="36"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="28" t="s">
         <v>39</v>
       </c>
@@ -1602,7 +1614,7 @@
       <c r="N11" s="3">
         <v>5</v>
       </c>
-      <c r="O11" s="36"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="28" t="s">
         <v>89</v>
       </c>
@@ -1617,7 +1629,7 @@
       <c r="G12" s="3">
         <v>3</v>
       </c>
-      <c r="H12" s="36"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="28" t="s">
         <v>40</v>
       </c>
@@ -1633,7 +1645,7 @@
       <c r="N12" s="3">
         <v>5</v>
       </c>
-      <c r="O12" s="36"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="28" t="s">
         <v>91</v>
       </c>
@@ -1648,7 +1660,7 @@
       <c r="G13" s="2">
         <v>3</v>
       </c>
-      <c r="H13" s="35">
+      <c r="H13" s="33">
         <v>28</v>
       </c>
       <c r="I13" s="20" t="s">
@@ -1664,7 +1676,7 @@
         <v>0.1</v>
       </c>
       <c r="N13" s="2"/>
-      <c r="O13" s="35">
+      <c r="O13" s="33">
         <v>28</v>
       </c>
       <c r="P13" s="20"/>
@@ -1677,7 +1689,7 @@
       <c r="G14" s="3">
         <v>3</v>
       </c>
-      <c r="H14" s="36"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="28" t="s">
         <v>65</v>
       </c>
@@ -1691,7 +1703,7 @@
         <v>0.1</v>
       </c>
       <c r="N14" s="3"/>
-      <c r="O14" s="36">
+      <c r="O14" s="34">
         <v>28</v>
       </c>
       <c r="P14" s="21"/>
@@ -1704,7 +1716,7 @@
       <c r="G15" s="3">
         <v>3</v>
       </c>
-      <c r="H15" s="36"/>
+      <c r="H15" s="34"/>
       <c r="I15" s="28" t="s">
         <v>66</v>
       </c>
@@ -1718,7 +1730,7 @@
         <v>0.1</v>
       </c>
       <c r="N15" s="3"/>
-      <c r="O15" s="36">
+      <c r="O15" s="34">
         <v>28</v>
       </c>
       <c r="P15" s="21"/>
@@ -1731,7 +1743,7 @@
       <c r="G16" s="3">
         <v>3</v>
       </c>
-      <c r="H16" s="36"/>
+      <c r="H16" s="34"/>
       <c r="I16" s="26" t="s">
         <v>73</v>
       </c>
@@ -1745,7 +1757,7 @@
         <v>0.1</v>
       </c>
       <c r="N16" s="3"/>
-      <c r="O16" s="36"/>
+      <c r="O16" s="34"/>
       <c r="P16" s="21"/>
       <c r="Q16" s="18"/>
       <c r="R16" s="3"/>
@@ -1756,7 +1768,7 @@
       <c r="G17" s="9">
         <v>3</v>
       </c>
-      <c r="H17" s="36"/>
+      <c r="H17" s="34"/>
       <c r="I17" s="26" t="s">
         <v>73</v>
       </c>
@@ -1770,7 +1782,7 @@
         <v>0.1</v>
       </c>
       <c r="N17" s="3"/>
-      <c r="O17" s="36"/>
+      <c r="O17" s="34"/>
       <c r="P17" s="21"/>
       <c r="Q17" s="18"/>
       <c r="R17" s="3"/>
@@ -1781,7 +1793,7 @@
       <c r="G18" s="3">
         <v>3</v>
       </c>
-      <c r="H18" s="36"/>
+      <c r="H18" s="34"/>
       <c r="I18" s="28" t="s">
         <v>76</v>
       </c>
@@ -1795,7 +1807,7 @@
         <v>0.1</v>
       </c>
       <c r="N18" s="3"/>
-      <c r="O18" s="36"/>
+      <c r="O18" s="34"/>
       <c r="P18" s="21"/>
       <c r="Q18" s="18"/>
       <c r="R18" s="3"/>
@@ -1806,7 +1818,7 @@
       <c r="G19" s="3">
         <v>3</v>
       </c>
-      <c r="H19" s="36"/>
+      <c r="H19" s="34"/>
       <c r="I19" s="28" t="s">
         <v>67</v>
       </c>
@@ -1820,7 +1832,7 @@
         <v>0.1</v>
       </c>
       <c r="N19" s="3"/>
-      <c r="O19" s="36"/>
+      <c r="O19" s="34"/>
       <c r="P19" s="21"/>
       <c r="Q19" s="18"/>
       <c r="R19" s="3"/>
@@ -1831,7 +1843,7 @@
       <c r="G20" s="3">
         <v>3</v>
       </c>
-      <c r="H20" s="36"/>
+      <c r="H20" s="34"/>
       <c r="I20" s="26" t="s">
         <v>73</v>
       </c>
@@ -1845,7 +1857,7 @@
         <v>0.1</v>
       </c>
       <c r="N20" s="3"/>
-      <c r="O20" s="36"/>
+      <c r="O20" s="34"/>
       <c r="P20" s="21"/>
       <c r="Q20" s="18"/>
       <c r="R20" s="3"/>
@@ -1856,7 +1868,7 @@
       <c r="G21" s="3">
         <v>3</v>
       </c>
-      <c r="H21" s="36"/>
+      <c r="H21" s="34"/>
       <c r="I21" s="28" t="s">
         <v>68</v>
       </c>
@@ -1870,7 +1882,7 @@
         <v>0.1</v>
       </c>
       <c r="N21" s="3"/>
-      <c r="O21" s="36"/>
+      <c r="O21" s="34"/>
       <c r="P21" s="21"/>
       <c r="Q21" s="18"/>
       <c r="R21" s="3"/>
@@ -1881,11 +1893,11 @@
       <c r="G22" s="3">
         <v>3</v>
       </c>
-      <c r="H22" s="38"/>
-      <c r="I22" s="43" t="s">
+      <c r="H22" s="36"/>
+      <c r="I22" s="41" t="s">
         <v>73</v>
       </c>
-      <c r="J22" s="44" t="s">
+      <c r="J22" s="42" t="s">
         <v>80</v>
       </c>
       <c r="L22" s="7" t="s">
@@ -1895,7 +1907,7 @@
         <v>0.1</v>
       </c>
       <c r="N22" s="4"/>
-      <c r="O22" s="38"/>
+      <c r="O22" s="36"/>
       <c r="P22" s="23"/>
       <c r="Q22" s="19"/>
       <c r="R22" s="4"/>
@@ -1913,13 +1925,13 @@
       <c r="C24" s="2">
         <v>7</v>
       </c>
-      <c r="D24" s="35" t="s">
+      <c r="D24" s="33" t="s">
         <v>81</v>
       </c>
-      <c r="E24" s="55" t="s">
+      <c r="E24" s="53" t="s">
         <v>73</v>
       </c>
-      <c r="F24" s="56">
+      <c r="F24" s="54">
         <v>1.0076000000000001</v>
       </c>
     </row>
@@ -1933,13 +1945,13 @@
       <c r="C25" s="3">
         <v>7</v>
       </c>
-      <c r="D25" s="36" t="s">
+      <c r="D25" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="E25" s="47" t="s">
+      <c r="E25" s="45" t="s">
         <v>45</v>
       </c>
-      <c r="F25" s="48" t="s">
+      <c r="F25" s="46" t="s">
         <v>82</v>
       </c>
     </row>
@@ -1953,13 +1965,13 @@
       <c r="C26" s="3">
         <v>7</v>
       </c>
-      <c r="D26" s="36" t="s">
+      <c r="D26" s="34" t="s">
         <v>81</v>
       </c>
-      <c r="E26" s="49" t="s">
+      <c r="E26" s="47" t="s">
         <v>47</v>
       </c>
-      <c r="F26" s="50" t="s">
+      <c r="F26" s="48" t="s">
         <v>83</v>
       </c>
     </row>
@@ -1973,11 +1985,11 @@
       <c r="C27" s="3">
         <v>7</v>
       </c>
-      <c r="D27" s="36"/>
-      <c r="E27" s="47" t="s">
+      <c r="D27" s="34"/>
+      <c r="E27" s="45" t="s">
         <v>49</v>
       </c>
-      <c r="F27" s="48" t="s">
+      <c r="F27" s="46" t="s">
         <v>84</v>
       </c>
     </row>
@@ -1991,11 +2003,11 @@
       <c r="C28" s="9">
         <v>7</v>
       </c>
-      <c r="D28" s="37"/>
-      <c r="E28" s="51" t="s">
+      <c r="D28" s="35"/>
+      <c r="E28" s="49" t="s">
         <v>51</v>
       </c>
-      <c r="F28" s="48" t="s">
+      <c r="F28" s="46" t="s">
         <v>85</v>
       </c>
     </row>
@@ -2009,11 +2021,11 @@
       <c r="C29" s="3">
         <v>7</v>
       </c>
-      <c r="D29" s="36"/>
-      <c r="E29" s="53" t="s">
+      <c r="D29" s="34"/>
+      <c r="E29" s="51" t="s">
         <v>73</v>
       </c>
-      <c r="F29" s="54">
+      <c r="F29" s="52">
         <v>1.0839000000000001</v>
       </c>
     </row>
@@ -2027,11 +2039,11 @@
       <c r="C30" s="3">
         <v>7</v>
       </c>
-      <c r="D30" s="36"/>
-      <c r="E30" s="47" t="s">
+      <c r="D30" s="34"/>
+      <c r="E30" s="45" t="s">
         <v>56</v>
       </c>
-      <c r="F30" s="48" t="s">
+      <c r="F30" s="46" t="s">
         <v>86</v>
       </c>
     </row>
@@ -2045,11 +2057,11 @@
       <c r="C31" s="3">
         <v>7</v>
       </c>
-      <c r="D31" s="36"/>
-      <c r="E31" s="47" t="s">
+      <c r="D31" s="34"/>
+      <c r="E31" s="45" t="s">
         <v>58</v>
       </c>
-      <c r="F31" s="48" t="s">
+      <c r="F31" s="46" t="s">
         <v>87</v>
       </c>
     </row>
@@ -2063,11 +2075,11 @@
       <c r="C32" s="3">
         <v>7</v>
       </c>
-      <c r="D32" s="36"/>
-      <c r="E32" s="47" t="s">
+      <c r="D32" s="34"/>
+      <c r="E32" s="45" t="s">
         <v>89</v>
       </c>
-      <c r="F32" s="48" t="s">
+      <c r="F32" s="46" t="s">
         <v>88</v>
       </c>
     </row>
@@ -2081,11 +2093,11 @@
       <c r="C33" s="3">
         <v>7</v>
       </c>
-      <c r="D33" s="36"/>
-      <c r="E33" s="47" t="s">
+      <c r="D33" s="34"/>
+      <c r="E33" s="45" t="s">
         <v>91</v>
       </c>
-      <c r="F33" s="48" t="s">
+      <c r="F33" s="46" t="s">
         <v>90</v>
       </c>
     </row>
@@ -2099,13 +2111,13 @@
       <c r="C34" s="2">
         <v>7</v>
       </c>
-      <c r="D34" s="35" t="s">
+      <c r="D34" s="33" t="s">
         <v>92</v>
       </c>
-      <c r="E34" s="45" t="s">
+      <c r="E34" s="43" t="s">
         <v>64</v>
       </c>
-      <c r="F34" s="46" t="s">
+      <c r="F34" s="44" t="s">
         <v>93</v>
       </c>
     </row>
@@ -2119,11 +2131,11 @@
       <c r="C35" s="3">
         <v>7</v>
       </c>
-      <c r="D35" s="36"/>
-      <c r="E35" s="47" t="s">
+      <c r="D35" s="34"/>
+      <c r="E35" s="45" t="s">
         <v>65</v>
       </c>
-      <c r="F35" s="48" t="s">
+      <c r="F35" s="46" t="s">
         <v>94</v>
       </c>
     </row>
@@ -2137,11 +2149,11 @@
       <c r="C36" s="3">
         <v>7</v>
       </c>
-      <c r="D36" s="36"/>
-      <c r="E36" s="47" t="s">
+      <c r="D36" s="34"/>
+      <c r="E36" s="45" t="s">
         <v>66</v>
       </c>
-      <c r="F36" s="48" t="s">
+      <c r="F36" s="46" t="s">
         <v>95</v>
       </c>
     </row>
@@ -2155,11 +2167,11 @@
       <c r="C37" s="3">
         <v>7</v>
       </c>
-      <c r="D37" s="36"/>
-      <c r="E37" s="49" t="s">
+      <c r="D37" s="34"/>
+      <c r="E37" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F37" s="50" t="s">
+      <c r="F37" s="48" t="s">
         <v>96</v>
       </c>
     </row>
@@ -2173,11 +2185,11 @@
       <c r="C38" s="9">
         <v>7</v>
       </c>
-      <c r="D38" s="36"/>
-      <c r="E38" s="49" t="s">
+      <c r="D38" s="34"/>
+      <c r="E38" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F38" s="50" t="s">
+      <c r="F38" s="48" t="s">
         <v>97</v>
       </c>
     </row>
@@ -2191,11 +2203,11 @@
       <c r="C39" s="3">
         <v>7</v>
       </c>
-      <c r="D39" s="36"/>
-      <c r="E39" s="49" t="s">
+      <c r="D39" s="34"/>
+      <c r="E39" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F39" s="50" t="s">
+      <c r="F39" s="48" t="s">
         <v>98</v>
       </c>
     </row>
@@ -2209,11 +2221,11 @@
       <c r="C40" s="3">
         <v>7</v>
       </c>
-      <c r="D40" s="36"/>
-      <c r="E40" s="47" t="s">
+      <c r="D40" s="34"/>
+      <c r="E40" s="45" t="s">
         <v>67</v>
       </c>
-      <c r="F40" s="48" t="s">
+      <c r="F40" s="46" t="s">
         <v>99</v>
       </c>
     </row>
@@ -2227,11 +2239,11 @@
       <c r="C41" s="3">
         <v>7</v>
       </c>
-      <c r="D41" s="36"/>
-      <c r="E41" s="49" t="s">
+      <c r="D41" s="34"/>
+      <c r="E41" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F41" s="50" t="s">
+      <c r="F41" s="48" t="s">
         <v>100</v>
       </c>
     </row>
@@ -2245,11 +2257,11 @@
       <c r="C42" s="3">
         <v>7</v>
       </c>
-      <c r="D42" s="36"/>
-      <c r="E42" s="47" t="s">
+      <c r="D42" s="34"/>
+      <c r="E42" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="F42" s="48" t="s">
+      <c r="F42" s="46" t="s">
         <v>101</v>
       </c>
     </row>
@@ -2263,11 +2275,11 @@
       <c r="C43" s="3">
         <v>7</v>
       </c>
-      <c r="D43" s="38"/>
-      <c r="E43" s="49" t="s">
+      <c r="D43" s="36"/>
+      <c r="E43" s="47" t="s">
         <v>73</v>
       </c>
-      <c r="F43" s="52" t="s">
+      <c r="F43" s="50" t="s">
         <v>102</v>
       </c>
     </row>
@@ -2285,10 +2297,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q25"/>
+  <dimension ref="A1:Q50"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L4" sqref="L4"/>
+    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+      <selection activeCell="M36" sqref="M36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
@@ -2303,10 +2315,10 @@
       <c r="C1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="32"/>
+      <c r="D1" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="65"/>
       <c r="G1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2316,10 +2328,10 @@
       <c r="I1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="J1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="K1" s="32"/>
+      <c r="J1" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="K1" s="65"/>
       <c r="M1" s="15" t="s">
         <v>0</v>
       </c>
@@ -2329,10 +2341,10 @@
       <c r="O1" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="P1" s="32" t="s">
-        <v>3</v>
-      </c>
-      <c r="Q1" s="32"/>
+      <c r="P1" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="Q1" s="65"/>
     </row>
     <row r="2" spans="1:17" ht="15.75" thickBot="1">
       <c r="A2" s="14"/>
@@ -2376,13 +2388,13 @@
       <c r="B3" s="2">
         <v>3</v>
       </c>
-      <c r="C3" s="35" t="s">
+      <c r="C3" s="33" t="s">
         <v>105</v>
       </c>
-      <c r="D3" s="58" t="s">
+      <c r="D3" s="56" t="s">
         <v>106</v>
       </c>
-      <c r="E3" s="59">
+      <c r="E3" s="57">
         <v>0.89580000000000004</v>
       </c>
       <c r="G3" s="5" t="s">
@@ -2391,7 +2403,7 @@
       <c r="H3" s="2">
         <v>5</v>
       </c>
-      <c r="I3" s="35" t="s">
+      <c r="I3" s="33" t="s">
         <v>114</v>
       </c>
       <c r="J3" s="20" t="s">
@@ -2400,20 +2412,20 @@
       <c r="K3" s="24">
         <v>0.98740000000000006</v>
       </c>
-      <c r="L3" s="66"/>
+      <c r="L3" s="64"/>
       <c r="M3" s="5" t="s">
         <v>4</v>
       </c>
       <c r="N3" s="2">
         <v>7</v>
       </c>
-      <c r="O3" s="35" t="s">
+      <c r="O3" s="33" t="s">
         <v>116</v>
       </c>
-      <c r="P3" s="64" t="s">
+      <c r="P3" s="62" t="s">
         <v>73</v>
       </c>
-      <c r="Q3" s="65">
+      <c r="Q3" s="63">
         <v>1.0082</v>
       </c>
     </row>
@@ -2436,7 +2448,7 @@
       <c r="H4" s="3">
         <v>5</v>
       </c>
-      <c r="I4" s="36" t="s">
+      <c r="I4" s="34" t="s">
         <v>114</v>
       </c>
       <c r="J4" s="28" t="s">
@@ -2451,7 +2463,7 @@
       <c r="N4" s="3">
         <v>7</v>
       </c>
-      <c r="O4" s="36"/>
+      <c r="O4" s="34"/>
       <c r="P4" s="30" t="s">
         <v>45</v>
       </c>
@@ -2466,7 +2478,7 @@
       <c r="B5" s="3">
         <v>3</v>
       </c>
-      <c r="C5" s="36"/>
+      <c r="C5" s="34"/>
       <c r="D5" s="30" t="s">
         <v>107</v>
       </c>
@@ -2479,7 +2491,7 @@
       <c r="H5" s="3">
         <v>5</v>
       </c>
-      <c r="I5" s="36"/>
+      <c r="I5" s="34"/>
       <c r="J5" s="30" t="s">
         <v>107</v>
       </c>
@@ -2492,7 +2504,7 @@
       <c r="N5" s="3">
         <v>7</v>
       </c>
-      <c r="O5" s="36"/>
+      <c r="O5" s="34"/>
       <c r="P5" s="30" t="s">
         <v>107</v>
       </c>
@@ -2507,7 +2519,7 @@
       <c r="B6" s="3">
         <v>3</v>
       </c>
-      <c r="C6" s="36"/>
+      <c r="C6" s="34"/>
       <c r="D6" s="30" t="s">
         <v>49</v>
       </c>
@@ -2520,7 +2532,7 @@
       <c r="H6" s="3">
         <v>5</v>
       </c>
-      <c r="I6" s="36"/>
+      <c r="I6" s="34"/>
       <c r="J6" s="30" t="s">
         <v>49</v>
       </c>
@@ -2533,7 +2545,7 @@
       <c r="N6" s="3">
         <v>7</v>
       </c>
-      <c r="O6" s="36"/>
+      <c r="O6" s="34"/>
       <c r="P6" s="30" t="s">
         <v>49</v>
       </c>
@@ -2548,8 +2560,8 @@
       <c r="B7" s="9">
         <v>3</v>
       </c>
-      <c r="C7" s="37"/>
-      <c r="D7" s="60" t="s">
+      <c r="C7" s="35"/>
+      <c r="D7" s="58" t="s">
         <v>51</v>
       </c>
       <c r="E7" s="31">
@@ -2561,7 +2573,7 @@
       <c r="H7" s="9">
         <v>5</v>
       </c>
-      <c r="I7" s="37"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="30" t="s">
         <v>51</v>
       </c>
@@ -2574,7 +2586,7 @@
       <c r="N7" s="9">
         <v>7</v>
       </c>
-      <c r="O7" s="37"/>
+      <c r="O7" s="35"/>
       <c r="P7" s="30" t="s">
         <v>51</v>
       </c>
@@ -2589,7 +2601,7 @@
       <c r="B8" s="3">
         <v>3</v>
       </c>
-      <c r="C8" s="36"/>
+      <c r="C8" s="34"/>
       <c r="D8" s="26" t="s">
         <v>53</v>
       </c>
@@ -2602,7 +2614,7 @@
       <c r="H8" s="3">
         <v>5</v>
       </c>
-      <c r="I8" s="36"/>
+      <c r="I8" s="34"/>
       <c r="J8" s="30" t="s">
         <v>73</v>
       </c>
@@ -2615,7 +2627,7 @@
       <c r="N8" s="3">
         <v>7</v>
       </c>
-      <c r="O8" s="36"/>
+      <c r="O8" s="34"/>
       <c r="P8" s="26" t="s">
         <v>73</v>
       </c>
@@ -2630,11 +2642,11 @@
       <c r="B9" s="3">
         <v>3</v>
       </c>
-      <c r="C9" s="36"/>
+      <c r="C9" s="34"/>
       <c r="D9" s="26" t="s">
         <v>108</v>
       </c>
-      <c r="E9" s="42">
+      <c r="E9" s="40">
         <v>0.84750000000000003</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -2643,7 +2655,7 @@
       <c r="H9" s="3">
         <v>5</v>
       </c>
-      <c r="I9" s="36"/>
+      <c r="I9" s="34"/>
       <c r="J9" s="26" t="s">
         <v>115</v>
       </c>
@@ -2656,7 +2668,7 @@
       <c r="N9" s="3">
         <v>7</v>
       </c>
-      <c r="O9" s="36"/>
+      <c r="O9" s="34"/>
       <c r="P9" s="26" t="s">
         <v>45</v>
       </c>
@@ -2671,7 +2683,7 @@
       <c r="B10" s="3">
         <v>3</v>
       </c>
-      <c r="C10" s="36"/>
+      <c r="C10" s="34"/>
       <c r="D10" s="30" t="s">
         <v>56</v>
       </c>
@@ -2684,7 +2696,7 @@
       <c r="H10" s="3">
         <v>5</v>
       </c>
-      <c r="I10" s="36"/>
+      <c r="I10" s="34"/>
       <c r="J10" s="30" t="s">
         <v>56</v>
       </c>
@@ -2697,7 +2709,7 @@
       <c r="N10" s="3">
         <v>7</v>
       </c>
-      <c r="O10" s="36"/>
+      <c r="O10" s="34"/>
       <c r="P10" s="30" t="s">
         <v>56</v>
       </c>
@@ -2712,7 +2724,7 @@
       <c r="B11" s="3">
         <v>3</v>
       </c>
-      <c r="C11" s="36"/>
+      <c r="C11" s="34"/>
       <c r="D11" s="30" t="s">
         <v>58</v>
       </c>
@@ -2725,7 +2737,7 @@
       <c r="H11" s="3">
         <v>5</v>
       </c>
-      <c r="I11" s="36"/>
+      <c r="I11" s="34"/>
       <c r="J11" s="30" t="s">
         <v>103</v>
       </c>
@@ -2738,7 +2750,7 @@
       <c r="N11" s="3">
         <v>7</v>
       </c>
-      <c r="O11" s="36"/>
+      <c r="O11" s="34"/>
       <c r="P11" s="30" t="s">
         <v>58</v>
       </c>
@@ -2753,7 +2765,7 @@
       <c r="B12" s="3">
         <v>3</v>
       </c>
-      <c r="C12" s="36"/>
+      <c r="C12" s="34"/>
       <c r="D12" s="30" t="s">
         <v>89</v>
       </c>
@@ -2766,7 +2778,7 @@
       <c r="H12" s="3">
         <v>5</v>
       </c>
-      <c r="I12" s="36"/>
+      <c r="I12" s="34"/>
       <c r="J12" s="30" t="s">
         <v>89</v>
       </c>
@@ -2779,7 +2791,7 @@
       <c r="N12" s="3">
         <v>7</v>
       </c>
-      <c r="O12" s="36"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="30" t="s">
         <v>89</v>
       </c>
@@ -2794,7 +2806,7 @@
       <c r="B13" s="3">
         <v>3</v>
       </c>
-      <c r="C13" s="36"/>
+      <c r="C13" s="34"/>
       <c r="D13" s="30" t="s">
         <v>91</v>
       </c>
@@ -2807,7 +2819,7 @@
       <c r="H13" s="3">
         <v>5</v>
       </c>
-      <c r="I13" s="36"/>
+      <c r="I13" s="34"/>
       <c r="J13" s="30" t="s">
         <v>91</v>
       </c>
@@ -2820,7 +2832,7 @@
       <c r="N13" s="3">
         <v>7</v>
       </c>
-      <c r="O13" s="36"/>
+      <c r="O13" s="34"/>
       <c r="P13" s="30" t="s">
         <v>91</v>
       </c>
@@ -2835,7 +2847,7 @@
       <c r="B14" s="3">
         <v>3</v>
       </c>
-      <c r="C14" s="36"/>
+      <c r="C14" s="34"/>
       <c r="D14" s="30" t="s">
         <v>64</v>
       </c>
@@ -2848,7 +2860,7 @@
       <c r="H14" s="3">
         <v>5</v>
       </c>
-      <c r="I14" s="36"/>
+      <c r="I14" s="34"/>
       <c r="J14" s="30" t="s">
         <v>64</v>
       </c>
@@ -2861,7 +2873,7 @@
       <c r="N14" s="3">
         <v>7</v>
       </c>
-      <c r="O14" s="36"/>
+      <c r="O14" s="34"/>
       <c r="P14" s="30" t="s">
         <v>64</v>
       </c>
@@ -2876,11 +2888,11 @@
       <c r="B15" s="3">
         <v>3</v>
       </c>
-      <c r="C15" s="36"/>
+      <c r="C15" s="34"/>
       <c r="D15" s="30" t="s">
         <v>65</v>
       </c>
-      <c r="E15" s="61">
+      <c r="E15" s="59">
         <v>0.44850000000000001</v>
       </c>
       <c r="G15" s="6" t="s">
@@ -2889,7 +2901,7 @@
       <c r="H15" s="3">
         <v>5</v>
       </c>
-      <c r="I15" s="36"/>
+      <c r="I15" s="34"/>
       <c r="J15" s="30" t="s">
         <v>65</v>
       </c>
@@ -2902,7 +2914,7 @@
       <c r="N15" s="3">
         <v>7</v>
       </c>
-      <c r="O15" s="36"/>
+      <c r="O15" s="34"/>
       <c r="P15" s="30" t="s">
         <v>65</v>
       </c>
@@ -2917,11 +2929,11 @@
       <c r="B16" s="3">
         <v>3</v>
       </c>
-      <c r="C16" s="36"/>
+      <c r="C16" s="34"/>
       <c r="D16" s="30" t="s">
         <v>66</v>
       </c>
-      <c r="E16" s="61">
+      <c r="E16" s="59">
         <v>0.43890000000000001</v>
       </c>
       <c r="G16" s="6" t="s">
@@ -2930,7 +2942,7 @@
       <c r="H16" s="3">
         <v>5</v>
       </c>
-      <c r="I16" s="36"/>
+      <c r="I16" s="34"/>
       <c r="J16" s="30" t="s">
         <v>66</v>
       </c>
@@ -2943,7 +2955,7 @@
       <c r="N16" s="3">
         <v>7</v>
       </c>
-      <c r="O16" s="36"/>
+      <c r="O16" s="34"/>
       <c r="P16" s="30" t="s">
         <v>66</v>
       </c>
@@ -2958,11 +2970,11 @@
       <c r="B17" s="3">
         <v>3</v>
       </c>
-      <c r="C17" s="36"/>
+      <c r="C17" s="34"/>
       <c r="D17" s="30" t="s">
         <v>109</v>
       </c>
-      <c r="E17" s="61">
+      <c r="E17" s="59">
         <v>0.56630000000000003</v>
       </c>
       <c r="G17" s="6" t="s">
@@ -2971,7 +2983,7 @@
       <c r="H17" s="3">
         <v>5</v>
       </c>
-      <c r="I17" s="36"/>
+      <c r="I17" s="34"/>
       <c r="J17" s="30" t="s">
         <v>109</v>
       </c>
@@ -2984,7 +2996,7 @@
       <c r="N17" s="3">
         <v>7</v>
       </c>
-      <c r="O17" s="36"/>
+      <c r="O17" s="34"/>
       <c r="P17" s="30" t="s">
         <v>109</v>
       </c>
@@ -2999,11 +3011,11 @@
       <c r="B18" s="9">
         <v>3</v>
       </c>
-      <c r="C18" s="36"/>
+      <c r="C18" s="34"/>
       <c r="D18" s="30" t="s">
         <v>110</v>
       </c>
-      <c r="E18" s="61">
+      <c r="E18" s="59">
         <v>0.54720000000000002</v>
       </c>
       <c r="G18" s="6" t="s">
@@ -3012,7 +3024,7 @@
       <c r="H18" s="9">
         <v>5</v>
       </c>
-      <c r="I18" s="36"/>
+      <c r="I18" s="34"/>
       <c r="J18" s="30" t="s">
         <v>110</v>
       </c>
@@ -3025,7 +3037,7 @@
       <c r="N18" s="9">
         <v>7</v>
       </c>
-      <c r="O18" s="36"/>
+      <c r="O18" s="34"/>
       <c r="P18" s="30" t="s">
         <v>110</v>
       </c>
@@ -3040,11 +3052,11 @@
       <c r="B19" s="3">
         <v>3</v>
       </c>
-      <c r="C19" s="36"/>
+      <c r="C19" s="34"/>
       <c r="D19" s="30" t="s">
         <v>76</v>
       </c>
-      <c r="E19" s="61">
+      <c r="E19" s="59">
         <v>0.443</v>
       </c>
       <c r="G19" s="6" t="s">
@@ -3053,7 +3065,7 @@
       <c r="H19" s="3">
         <v>5</v>
       </c>
-      <c r="I19" s="36"/>
+      <c r="I19" s="34"/>
       <c r="J19" s="30" t="s">
         <v>76</v>
       </c>
@@ -3066,7 +3078,7 @@
       <c r="N19" s="3">
         <v>7</v>
       </c>
-      <c r="O19" s="36"/>
+      <c r="O19" s="34"/>
       <c r="P19" s="30" t="s">
         <v>76</v>
       </c>
@@ -3081,11 +3093,11 @@
       <c r="B20" s="3">
         <v>3</v>
       </c>
-      <c r="C20" s="36"/>
+      <c r="C20" s="34"/>
       <c r="D20" s="30" t="s">
         <v>67</v>
       </c>
-      <c r="E20" s="61">
+      <c r="E20" s="59">
         <v>0.14149999999999999</v>
       </c>
       <c r="G20" s="6" t="s">
@@ -3094,7 +3106,7 @@
       <c r="H20" s="3">
         <v>5</v>
       </c>
-      <c r="I20" s="36"/>
+      <c r="I20" s="34"/>
       <c r="J20" s="30" t="s">
         <v>67</v>
       </c>
@@ -3107,7 +3119,7 @@
       <c r="N20" s="3">
         <v>7</v>
       </c>
-      <c r="O20" s="36"/>
+      <c r="O20" s="34"/>
       <c r="P20" s="30" t="s">
         <v>67</v>
       </c>
@@ -3122,11 +3134,11 @@
       <c r="B21" s="3">
         <v>3</v>
       </c>
-      <c r="C21" s="36"/>
+      <c r="C21" s="34"/>
       <c r="D21" s="30" t="s">
         <v>111</v>
       </c>
-      <c r="E21" s="61">
+      <c r="E21" s="59">
         <v>0.71789999999999998</v>
       </c>
       <c r="G21" s="6" t="s">
@@ -3135,7 +3147,7 @@
       <c r="H21" s="3">
         <v>5</v>
       </c>
-      <c r="I21" s="36"/>
+      <c r="I21" s="34"/>
       <c r="J21" s="30" t="s">
         <v>111</v>
       </c>
@@ -3148,7 +3160,7 @@
       <c r="N21" s="3">
         <v>7</v>
       </c>
-      <c r="O21" s="36"/>
+      <c r="O21" s="34"/>
       <c r="P21" s="30" t="s">
         <v>111</v>
       </c>
@@ -3163,11 +3175,11 @@
       <c r="B22" s="3">
         <v>3</v>
       </c>
-      <c r="C22" s="36"/>
+      <c r="C22" s="34"/>
       <c r="D22" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="E22" s="61">
+      <c r="E22" s="59">
         <v>0.38</v>
       </c>
       <c r="G22" s="6" t="s">
@@ -3176,7 +3188,7 @@
       <c r="H22" s="3">
         <v>5</v>
       </c>
-      <c r="I22" s="36"/>
+      <c r="I22" s="34"/>
       <c r="J22" s="30" t="s">
         <v>68</v>
       </c>
@@ -3189,7 +3201,7 @@
       <c r="N22" s="3">
         <v>7</v>
       </c>
-      <c r="O22" s="36"/>
+      <c r="O22" s="34"/>
       <c r="P22" s="30" t="s">
         <v>68</v>
       </c>
@@ -3204,11 +3216,11 @@
       <c r="B23" s="3">
         <v>3</v>
       </c>
-      <c r="C23" s="38"/>
-      <c r="D23" s="62" t="s">
+      <c r="C23" s="36"/>
+      <c r="D23" s="60" t="s">
         <v>112</v>
       </c>
-      <c r="E23" s="63">
+      <c r="E23" s="61">
         <v>0.55000000000000004</v>
       </c>
       <c r="G23" s="7" t="s">
@@ -3217,7 +3229,7 @@
       <c r="H23" s="3">
         <v>5</v>
       </c>
-      <c r="I23" s="38"/>
+      <c r="I23" s="36"/>
       <c r="J23" s="30" t="s">
         <v>112</v>
       </c>
@@ -3230,7 +3242,7 @@
       <c r="N23" s="3">
         <v>7</v>
       </c>
-      <c r="O23" s="38"/>
+      <c r="O23" s="36"/>
       <c r="P23" s="30" t="s">
         <v>112</v>
       </c>
@@ -3239,17 +3251,718 @@
       </c>
     </row>
     <row r="25" spans="1:17">
-      <c r="A25" s="57" t="s">
+      <c r="A25" s="55" t="s">
         <v>104</v>
       </c>
     </row>
+    <row r="27" spans="1:17">
+      <c r="A27" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="B27">
+        <v>0.5</v>
+      </c>
+      <c r="H27" s="55" t="s">
+        <v>117</v>
+      </c>
+      <c r="I27">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17">
+      <c r="A28" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="D28" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="E28" s="65"/>
+      <c r="H28" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>2</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="K28" s="65" t="s">
+        <v>3</v>
+      </c>
+      <c r="L28" s="65"/>
+    </row>
+    <row r="29" spans="1:17" ht="15.75" thickBot="1">
+      <c r="A29" s="32"/>
+      <c r="B29" s="32"/>
+      <c r="C29" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="D29" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>1</v>
+      </c>
+      <c r="H29" s="32"/>
+      <c r="I29" s="32"/>
+      <c r="J29" s="32" t="s">
+        <v>42</v>
+      </c>
+      <c r="K29" s="32" t="s">
+        <v>0</v>
+      </c>
+      <c r="L29" s="32" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17">
+      <c r="A30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B30" s="2">
+        <v>3</v>
+      </c>
+      <c r="C30" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="D30" s="68" t="str">
+        <f>IF(E30&lt;0.5,D3,"N E")</f>
+        <v>N E</v>
+      </c>
+      <c r="E30" s="63">
+        <v>0.89580000000000004</v>
+      </c>
+      <c r="H30" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="I30" s="2">
+        <v>3</v>
+      </c>
+      <c r="J30" s="33" t="s">
+        <v>105</v>
+      </c>
+      <c r="K30" s="68" t="str">
+        <f>IF(L30&lt;0.75,D3,"N E")</f>
+        <v>N E</v>
+      </c>
+      <c r="L30" s="63">
+        <v>0.89580000000000004</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17">
+      <c r="A31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B31" s="3">
+        <v>3</v>
+      </c>
+      <c r="D31" s="56" t="str">
+        <f t="shared" ref="D31:D50" si="0">IF(E31&lt;0.5,D4,"N E")</f>
+        <v>s03\09</v>
+      </c>
+      <c r="E31" s="31">
+        <v>0.378</v>
+      </c>
+      <c r="H31" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="3">
+        <v>3</v>
+      </c>
+      <c r="K31" s="56" t="str">
+        <f>IF(L31&lt;0.75,D4,"N E")</f>
+        <v>s03\09</v>
+      </c>
+      <c r="L31" s="31">
+        <v>0.378</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17">
+      <c r="A32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="B32" s="3">
+        <v>3</v>
+      </c>
+      <c r="C32" s="34"/>
+      <c r="D32" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s05\06</v>
+      </c>
+      <c r="E32" s="31">
+        <v>0.25019999999999998</v>
+      </c>
+      <c r="H32" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="I32" s="3">
+        <v>3</v>
+      </c>
+      <c r="J32" s="34"/>
+      <c r="K32" s="56" t="str">
+        <f t="shared" ref="K32:K50" si="1">IF(L32&lt;0.75,D5,"N E")</f>
+        <v>s05\06</v>
+      </c>
+      <c r="L32" s="31">
+        <v>0.25019999999999998</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12">
+      <c r="A33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="3">
+        <v>3</v>
+      </c>
+      <c r="C33" s="34"/>
+      <c r="D33" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E33" s="27">
+        <v>0.55489999999999995</v>
+      </c>
+      <c r="H33" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="I33" s="3">
+        <v>3</v>
+      </c>
+      <c r="J33" s="34"/>
+      <c r="K33" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s07\05</v>
+      </c>
+      <c r="L33" s="27">
+        <v>0.55489999999999995</v>
+      </c>
+    </row>
+    <row r="34" spans="1:12">
+      <c r="A34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" s="9">
+        <v>3</v>
+      </c>
+      <c r="C34" s="35"/>
+      <c r="D34" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E34" s="27">
+        <v>0.59499999999999997</v>
+      </c>
+      <c r="H34" s="8" t="s">
+        <v>8</v>
+      </c>
+      <c r="I34" s="9">
+        <v>3</v>
+      </c>
+      <c r="J34" s="35"/>
+      <c r="K34" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s09\05</v>
+      </c>
+      <c r="L34" s="27">
+        <v>0.59499999999999997</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12">
+      <c r="A35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="B35" s="3">
+        <v>3</v>
+      </c>
+      <c r="C35" s="34"/>
+      <c r="D35" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E35" s="27">
+        <v>0.99680000000000002</v>
+      </c>
+      <c r="H35" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="I35" s="3">
+        <v>3</v>
+      </c>
+      <c r="J35" s="34"/>
+      <c r="K35" s="68" t="str">
+        <f t="shared" si="1"/>
+        <v>N E</v>
+      </c>
+      <c r="L35" s="27">
+        <v>0.99680000000000002</v>
+      </c>
+    </row>
+    <row r="36" spans="1:12">
+      <c r="A36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="B36" s="3">
+        <v>3</v>
+      </c>
+      <c r="C36" s="34"/>
+      <c r="D36" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E36" s="40">
+        <v>0.84750000000000003</v>
+      </c>
+      <c r="H36" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="I36" s="3">
+        <v>3</v>
+      </c>
+      <c r="J36" s="34"/>
+      <c r="K36" s="68" t="str">
+        <f t="shared" si="1"/>
+        <v>N E</v>
+      </c>
+      <c r="L36" s="40">
+        <v>0.84750000000000003</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12">
+      <c r="A37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B37" s="3">
+        <v>3</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s13\05</v>
+      </c>
+      <c r="E37" s="31">
+        <v>0.2445</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="I37" s="3">
+        <v>3</v>
+      </c>
+      <c r="J37" s="34"/>
+      <c r="K37" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s13\05</v>
+      </c>
+      <c r="L37" s="31">
+        <v>0.2445</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12">
+      <c r="A38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="B38" s="3">
+        <v>3</v>
+      </c>
+      <c r="C38" s="34"/>
+      <c r="D38" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s15\05</v>
+      </c>
+      <c r="E38" s="31">
+        <v>0.3427</v>
+      </c>
+      <c r="H38" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="I38" s="3">
+        <v>3</v>
+      </c>
+      <c r="J38" s="34"/>
+      <c r="K38" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s15\05</v>
+      </c>
+      <c r="L38" s="31">
+        <v>0.3427</v>
+      </c>
+    </row>
+    <row r="39" spans="1:12">
+      <c r="A39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="B39" s="3">
+        <v>3</v>
+      </c>
+      <c r="C39" s="34"/>
+      <c r="D39" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s17\07</v>
+      </c>
+      <c r="E39" s="31">
+        <v>0.36859999999999998</v>
+      </c>
+      <c r="H39" s="6" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" s="3">
+        <v>3</v>
+      </c>
+      <c r="J39" s="34"/>
+      <c r="K39" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s17\07</v>
+      </c>
+      <c r="L39" s="31">
+        <v>0.36859999999999998</v>
+      </c>
+    </row>
+    <row r="40" spans="1:12">
+      <c r="A40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="B40" s="3">
+        <v>3</v>
+      </c>
+      <c r="C40" s="34"/>
+      <c r="D40" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s19\01</v>
+      </c>
+      <c r="E40" s="31">
+        <v>0.46829999999999999</v>
+      </c>
+      <c r="H40" s="6" t="s">
+        <v>12</v>
+      </c>
+      <c r="I40" s="3">
+        <v>3</v>
+      </c>
+      <c r="J40" s="34"/>
+      <c r="K40" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s19\01</v>
+      </c>
+      <c r="L40" s="31">
+        <v>0.46829999999999999</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12">
+      <c r="A41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="B41" s="3">
+        <v>3</v>
+      </c>
+      <c r="C41" s="34"/>
+      <c r="D41" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s21\08</v>
+      </c>
+      <c r="E41" s="31">
+        <v>0.3569</v>
+      </c>
+      <c r="H41" s="6" t="s">
+        <v>13</v>
+      </c>
+      <c r="I41" s="3">
+        <v>3</v>
+      </c>
+      <c r="J41" s="34"/>
+      <c r="K41" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s21\08</v>
+      </c>
+      <c r="L41" s="31">
+        <v>0.3569</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12">
+      <c r="A42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B42" s="3">
+        <v>3</v>
+      </c>
+      <c r="C42" s="34"/>
+      <c r="D42" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s23\01</v>
+      </c>
+      <c r="E42" s="59">
+        <v>0.44850000000000001</v>
+      </c>
+      <c r="H42" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="I42" s="3">
+        <v>3</v>
+      </c>
+      <c r="J42" s="34"/>
+      <c r="K42" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s23\01</v>
+      </c>
+      <c r="L42" s="59">
+        <v>0.44850000000000001</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12">
+      <c r="A43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="B43" s="3">
+        <v>3</v>
+      </c>
+      <c r="C43" s="34"/>
+      <c r="D43" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s25\03</v>
+      </c>
+      <c r="E43" s="59">
+        <v>0.43890000000000001</v>
+      </c>
+      <c r="H43" s="6" t="s">
+        <v>15</v>
+      </c>
+      <c r="I43" s="3">
+        <v>3</v>
+      </c>
+      <c r="J43" s="34"/>
+      <c r="K43" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s25\03</v>
+      </c>
+      <c r="L43" s="59">
+        <v>0.43890000000000001</v>
+      </c>
+    </row>
+    <row r="44" spans="1:12">
+      <c r="A44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="B44" s="3">
+        <v>3</v>
+      </c>
+      <c r="C44" s="34"/>
+      <c r="D44" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E44" s="40">
+        <v>0.56630000000000003</v>
+      </c>
+      <c r="H44" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="I44" s="3">
+        <v>3</v>
+      </c>
+      <c r="J44" s="34"/>
+      <c r="K44" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s27\01</v>
+      </c>
+      <c r="L44" s="40">
+        <v>0.56630000000000003</v>
+      </c>
+    </row>
+    <row r="45" spans="1:12">
+      <c r="A45" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="B45" s="9">
+        <v>3</v>
+      </c>
+      <c r="C45" s="34"/>
+      <c r="D45" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E45" s="40">
+        <v>0.54720000000000002</v>
+      </c>
+      <c r="H45" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="I45" s="9">
+        <v>3</v>
+      </c>
+      <c r="J45" s="34"/>
+      <c r="K45" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s29\03</v>
+      </c>
+      <c r="L45" s="40">
+        <v>0.54720000000000002</v>
+      </c>
+    </row>
+    <row r="46" spans="1:12">
+      <c r="A46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="B46" s="3">
+        <v>3</v>
+      </c>
+      <c r="C46" s="34"/>
+      <c r="D46" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s31\05</v>
+      </c>
+      <c r="E46" s="59">
+        <v>0.443</v>
+      </c>
+      <c r="H46" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="I46" s="3">
+        <v>3</v>
+      </c>
+      <c r="J46" s="34"/>
+      <c r="K46" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s31\05</v>
+      </c>
+      <c r="L46" s="59">
+        <v>0.443</v>
+      </c>
+    </row>
+    <row r="47" spans="1:12">
+      <c r="A47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="B47" s="3">
+        <v>3</v>
+      </c>
+      <c r="C47" s="34"/>
+      <c r="D47" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s33\02</v>
+      </c>
+      <c r="E47" s="59">
+        <v>0.14149999999999999</v>
+      </c>
+      <c r="H47" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="I47" s="3">
+        <v>3</v>
+      </c>
+      <c r="J47" s="34"/>
+      <c r="K47" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s33\02</v>
+      </c>
+      <c r="L47" s="59">
+        <v>0.14149999999999999</v>
+      </c>
+    </row>
+    <row r="48" spans="1:12">
+      <c r="A48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="B48" s="3">
+        <v>3</v>
+      </c>
+      <c r="C48" s="34"/>
+      <c r="D48" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E48" s="40">
+        <v>0.71789999999999998</v>
+      </c>
+      <c r="H48" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I48" s="3">
+        <v>3</v>
+      </c>
+      <c r="J48" s="34"/>
+      <c r="K48" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s35\05</v>
+      </c>
+      <c r="L48" s="40">
+        <v>0.71789999999999998</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12">
+      <c r="A49" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B49" s="3">
+        <v>3</v>
+      </c>
+      <c r="C49" s="34"/>
+      <c r="D49" s="56" t="str">
+        <f t="shared" si="0"/>
+        <v>s37\09</v>
+      </c>
+      <c r="E49" s="59">
+        <v>0.38</v>
+      </c>
+      <c r="H49" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="I49" s="3">
+        <v>3</v>
+      </c>
+      <c r="J49" s="34"/>
+      <c r="K49" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s37\09</v>
+      </c>
+      <c r="L49" s="59">
+        <v>0.38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:12" ht="15.75" thickBot="1">
+      <c r="A50" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="B50" s="3">
+        <v>3</v>
+      </c>
+      <c r="C50" s="36"/>
+      <c r="D50" s="68" t="str">
+        <f t="shared" si="0"/>
+        <v>N E</v>
+      </c>
+      <c r="E50" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="H50" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="I50" s="3">
+        <v>3</v>
+      </c>
+      <c r="J50" s="36"/>
+      <c r="K50" s="56" t="str">
+        <f t="shared" si="1"/>
+        <v>s39\06</v>
+      </c>
+      <c r="L50" s="69">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="3">
+  <mergeCells count="5">
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="J1:K1"/>
     <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="D28:E28"/>
+    <mergeCell ref="K28:L28"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>